<commit_message>
Updated Scrum Board for Sprint 2
</commit_message>
<xml_diff>
--- a/info/SCRUM_board.xlsx
+++ b/info/SCRUM_board.xlsx
@@ -158,9 +158,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -172,6 +169,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,7 +524,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -536,179 +536,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update Scrum Board for Sprint 3
</commit_message>
<xml_diff>
--- a/info/SCRUM_board.xlsx
+++ b/info/SCRUM_board.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>SCRUM Board</t>
   </si>
@@ -33,37 +33,31 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Have an aesthetically pleasing way of displaying costs</t>
-  </si>
-  <si>
-    <t>Find a way to upload pictures to the website</t>
-  </si>
-  <si>
-    <t>Make the picture accessible to everyone who is splitting payment</t>
-  </si>
-  <si>
-    <t>Come up with the best method to store user information</t>
-  </si>
-  <si>
-    <t>Write a separate method to divide costs by percentage</t>
-  </si>
-  <si>
-    <t>Figure out how to send a text or email notifications over web apps</t>
-  </si>
-  <si>
-    <t>Write a function that divides costs</t>
-  </si>
-  <si>
-    <t>Integrate the Facebook JavaScript sdk</t>
-  </si>
-  <si>
-    <t>Test the website to find the best location for Facebook integration</t>
-  </si>
-  <si>
-    <t>Begin implementing whatever we come up with</t>
-  </si>
-  <si>
-    <t>Implement notification functionality</t>
+    <t xml:space="preserve">Generate a Venmo URL that can be used to charge everyone </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use the amount of people to generate an editable form </t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a stopgap, use a student website that we are all provided with </t>
+  </si>
+  <si>
+    <t>Update the cost divide function to calculate a variable cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate a Venmo URL for each user with variable cost </t>
+  </si>
+  <si>
+    <t>Make sure appropriate values are entered in the initial form</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In a custom split, make sure the custom split adds up to the total amount </t>
+  </si>
+  <si>
+    <t>Somehow attempt to verity that the Venmo usernames are legitimate</t>
+  </si>
+  <si>
+    <t>Make the editable form of Venmo usernames also have a field for the %</t>
   </si>
 </sst>
 </file>
@@ -156,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,6 +167,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,12 +519,12 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="1" max="1" width="61.42578125" customWidth="1"/>
     <col min="2" max="2" width="27.7109375"/>
     <col min="3" max="3" width="34.28515625"/>
     <col min="4" max="1025" width="11.5703125"/>
@@ -554,71 +549,75 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="B11" s="4"/>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" s="4"/>
-      <c r="C12" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
@@ -705,7 +704,7 @@
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>